<commit_message>
Excel Data, Config Data, Test SUCCESS
</commit_message>
<xml_diff>
--- a/MavenFrame/TestData/Data.xlsx
+++ b/MavenFrame/TestData/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFD330A-885C-4B6F-9B9B-F622BF81468B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B26A93-A5AF-49DD-8892-E01EC8C08C73}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>takiastab2@gmail.com</t>
   </si>
   <si>
-    <t>makali@17</t>
-  </si>
-  <si>
-    <t>mesaikat17@gmail.com</t>
+    <t>makali17</t>
   </si>
 </sst>
 </file>
@@ -349,7 +346,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -368,19 +365,14 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{C62A570B-1270-4D84-91B8-B09C8870DBBB}"/>
-    <hyperlink ref="B1" r:id="rId2" xr:uid="{A368D8CA-539C-4BDD-A4AA-B6184A3C910F}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{0B142D5B-7CE4-45FB-B78F-3A9E39CEFE79}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{EA998BEC-240B-42E6-AC6F-9F8AC3E35C38}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>